<commit_message>
Fixing the Volue data fetching error
</commit_message>
<xml_diff>
--- a/Market Fundamentals/Entsoe_data/Load_Forecast.xlsx
+++ b/Market Fundamentals/Entsoe_data/Load_Forecast.xlsx
@@ -397,778 +397,778 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2">
-        <v>45424</v>
+        <v>45427</v>
       </c>
       <c r="B2">
-        <v>5000</v>
+        <v>5380</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2">
-        <v>45424.01041666666</v>
+        <v>45427.01041666666</v>
       </c>
       <c r="B3">
-        <v>4950</v>
+        <v>5340</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2">
-        <v>45424.02083333334</v>
+        <v>45427.02083333334</v>
       </c>
       <c r="B4">
-        <v>4900</v>
+        <v>5300</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2">
-        <v>45424.03125</v>
+        <v>45427.03125</v>
       </c>
       <c r="B5">
-        <v>4850</v>
+        <v>5260</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2">
-        <v>45424.04166666666</v>
+        <v>45427.04166666666</v>
       </c>
       <c r="B6">
-        <v>4800</v>
+        <v>5230</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2">
-        <v>45424.05208333334</v>
+        <v>45427.05208333334</v>
       </c>
       <c r="B7">
-        <v>4760</v>
+        <v>5210</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2">
-        <v>45424.0625</v>
+        <v>45427.0625</v>
       </c>
       <c r="B8">
-        <v>4730</v>
+        <v>5190</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2">
-        <v>45424.07291666666</v>
+        <v>45427.07291666666</v>
       </c>
       <c r="B9">
-        <v>4710</v>
+        <v>5160</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2">
-        <v>45424.08333333334</v>
+        <v>45427.08333333334</v>
       </c>
       <c r="B10">
-        <v>4700</v>
+        <v>5120</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2">
-        <v>45424.09375</v>
+        <v>45427.09375</v>
       </c>
       <c r="B11">
-        <v>4690</v>
+        <v>5100</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2">
-        <v>45424.10416666666</v>
+        <v>45427.10416666666</v>
       </c>
       <c r="B12">
-        <v>4680</v>
+        <v>5100</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2">
-        <v>45424.11458333334</v>
+        <v>45427.11458333334</v>
       </c>
       <c r="B13">
-        <v>4680</v>
+        <v>5110</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2">
-        <v>45424.125</v>
+        <v>45427.125</v>
       </c>
       <c r="B14">
-        <v>4680</v>
+        <v>5130</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2">
-        <v>45424.13541666666</v>
+        <v>45427.13541666666</v>
       </c>
       <c r="B15">
-        <v>4680</v>
+        <v>5150</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="2">
-        <v>45424.14583333334</v>
+        <v>45427.14583333334</v>
       </c>
       <c r="B16">
-        <v>4670</v>
+        <v>5160</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="2">
-        <v>45424.15625</v>
+        <v>45427.15625</v>
       </c>
       <c r="B17">
-        <v>4670</v>
+        <v>5170</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="2">
-        <v>45424.16666666666</v>
+        <v>45427.16666666666</v>
       </c>
       <c r="B18">
-        <v>4670</v>
+        <v>5190</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2">
-        <v>45424.17708333334</v>
+        <v>45427.17708333334</v>
       </c>
       <c r="B19">
-        <v>4670</v>
+        <v>5220</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2">
-        <v>45424.1875</v>
+        <v>45427.1875</v>
       </c>
       <c r="B20">
-        <v>4670</v>
+        <v>5260</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="2">
-        <v>45424.19791666666</v>
+        <v>45427.19791666666</v>
       </c>
       <c r="B21">
-        <v>4670</v>
+        <v>5330</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="2">
-        <v>45424.20833333334</v>
+        <v>45427.20833333334</v>
       </c>
       <c r="B22">
-        <v>4670</v>
+        <v>5420</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="2">
-        <v>45424.21875</v>
+        <v>45427.21875</v>
       </c>
       <c r="B23">
-        <v>4680</v>
+        <v>5520</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="2">
-        <v>45424.22916666666</v>
+        <v>45427.22916666666</v>
       </c>
       <c r="B24">
-        <v>4690</v>
+        <v>5620</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2">
-        <v>45424.23958333334</v>
+        <v>45427.23958333334</v>
       </c>
       <c r="B25">
-        <v>4700</v>
+        <v>5750</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2">
-        <v>45424.25</v>
+        <v>45427.25</v>
       </c>
       <c r="B26">
-        <v>4720</v>
+        <v>5900</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2">
-        <v>45424.26041666666</v>
+        <v>45427.26041666666</v>
       </c>
       <c r="B27">
-        <v>4750</v>
+        <v>6030</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2">
-        <v>45424.27083333334</v>
+        <v>45427.27083333334</v>
       </c>
       <c r="B28">
-        <v>4770</v>
+        <v>6110</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="2">
-        <v>45424.28125</v>
+        <v>45427.28125</v>
       </c>
       <c r="B29">
-        <v>4800</v>
+        <v>6160</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="2">
-        <v>45424.29166666666</v>
+        <v>45427.29166666666</v>
       </c>
       <c r="B30">
-        <v>4820</v>
+        <v>6180</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2">
-        <v>45424.30208333334</v>
+        <v>45427.30208333334</v>
       </c>
       <c r="B31">
-        <v>4840</v>
+        <v>6180</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2">
-        <v>45424.3125</v>
+        <v>45427.3125</v>
       </c>
       <c r="B32">
-        <v>4850</v>
+        <v>6170</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="2">
-        <v>45424.32291666666</v>
+        <v>45427.32291666666</v>
       </c>
       <c r="B33">
-        <v>4850</v>
+        <v>6140</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="2">
-        <v>45424.33333333334</v>
+        <v>45427.33333333334</v>
       </c>
       <c r="B34">
-        <v>4830</v>
+        <v>6060</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="2">
-        <v>45424.34375</v>
+        <v>45427.34375</v>
       </c>
       <c r="B35">
-        <v>4790</v>
+        <v>5970</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="2">
-        <v>45424.35416666666</v>
+        <v>45427.35416666666</v>
       </c>
       <c r="B36">
-        <v>4750</v>
+        <v>5880</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2">
-        <v>45424.36458333334</v>
+        <v>45427.36458333334</v>
       </c>
       <c r="B37">
-        <v>4700</v>
+        <v>5780</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2">
-        <v>45424.375</v>
+        <v>45427.375</v>
       </c>
       <c r="B38">
-        <v>4640</v>
+        <v>5710</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="2">
-        <v>45424.38541666666</v>
+        <v>45427.38541666666</v>
       </c>
       <c r="B39">
-        <v>4590</v>
+        <v>5630</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2">
-        <v>45424.39583333334</v>
+        <v>45427.39583333334</v>
       </c>
       <c r="B40">
-        <v>4540</v>
+        <v>5560</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="2">
-        <v>45424.40625</v>
+        <v>45427.40625</v>
       </c>
       <c r="B41">
-        <v>4490</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="2">
-        <v>45424.41666666666</v>
+        <v>45427.41666666666</v>
       </c>
       <c r="B42">
-        <v>4460</v>
+        <v>5440</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="2">
-        <v>45424.42708333334</v>
+        <v>45427.42708333334</v>
       </c>
       <c r="B43">
-        <v>4440</v>
+        <v>5420</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="2">
-        <v>45424.4375</v>
+        <v>45427.4375</v>
       </c>
       <c r="B44">
-        <v>4420</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="2">
-        <v>45424.44791666666</v>
+        <v>45427.44791666666</v>
       </c>
       <c r="B45">
-        <v>4410</v>
+        <v>5390</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2">
-        <v>45424.45833333334</v>
+        <v>45427.45833333334</v>
       </c>
       <c r="B46">
-        <v>4410</v>
+        <v>5380</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2">
-        <v>45424.46875</v>
+        <v>45427.46875</v>
       </c>
       <c r="B47">
-        <v>4400</v>
+        <v>5380</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="2">
-        <v>45424.47916666666</v>
+        <v>45427.47916666666</v>
       </c>
       <c r="B48">
-        <v>4390</v>
+        <v>5380</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="2">
-        <v>45424.48958333334</v>
+        <v>45427.48958333334</v>
       </c>
       <c r="B49">
-        <v>4380</v>
+        <v>5380</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="2">
-        <v>45424.5</v>
+        <v>45427.5</v>
       </c>
       <c r="B50">
-        <v>4360</v>
+        <v>5390</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="2">
-        <v>45424.51041666666</v>
+        <v>45427.51041666666</v>
       </c>
       <c r="B51">
-        <v>4350</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="2">
-        <v>45424.52083333334</v>
+        <v>45427.52083333334</v>
       </c>
       <c r="B52">
-        <v>4340</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="2">
-        <v>45424.53125</v>
+        <v>45427.53125</v>
       </c>
       <c r="B53">
-        <v>4330</v>
+        <v>5380</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="2">
-        <v>45424.54166666666</v>
+        <v>45427.54166666666</v>
       </c>
       <c r="B54">
-        <v>4330</v>
+        <v>5340</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="2">
-        <v>45424.55208333334</v>
+        <v>45427.55208333334</v>
       </c>
       <c r="B55">
-        <v>4330</v>
+        <v>5320</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="2">
-        <v>45424.5625</v>
+        <v>45427.5625</v>
       </c>
       <c r="B56">
-        <v>4340</v>
+        <v>5310</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="2">
-        <v>45424.57291666666</v>
+        <v>45427.57291666666</v>
       </c>
       <c r="B57">
-        <v>4340</v>
+        <v>5310</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="2">
-        <v>45424.58333333334</v>
+        <v>45427.58333333334</v>
       </c>
       <c r="B58">
-        <v>4360</v>
+        <v>5310</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="2">
-        <v>45424.59375</v>
+        <v>45427.59375</v>
       </c>
       <c r="B59">
-        <v>4370</v>
+        <v>5310</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="2">
-        <v>45424.60416666666</v>
+        <v>45427.60416666666</v>
       </c>
       <c r="B60">
-        <v>4390</v>
+        <v>5320</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="2">
-        <v>45424.61458333334</v>
+        <v>45427.61458333334</v>
       </c>
       <c r="B61">
-        <v>4410</v>
+        <v>5340</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="2">
-        <v>45424.625</v>
+        <v>45427.625</v>
       </c>
       <c r="B62">
-        <v>4440</v>
+        <v>5390</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="2">
-        <v>45424.63541666666</v>
+        <v>45427.63541666666</v>
       </c>
       <c r="B63">
-        <v>4490</v>
+        <v>5450</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="2">
-        <v>45424.64583333334</v>
+        <v>45427.64583333334</v>
       </c>
       <c r="B64">
-        <v>4550</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="2">
-        <v>45424.65625</v>
+        <v>45427.65625</v>
       </c>
       <c r="B65">
-        <v>4620</v>
+        <v>5560</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="2">
-        <v>45424.66666666666</v>
+        <v>45427.66666666666</v>
       </c>
       <c r="B66">
-        <v>4690</v>
+        <v>5610</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="2">
-        <v>45424.67708333334</v>
+        <v>45427.67708333334</v>
       </c>
       <c r="B67">
-        <v>4770</v>
+        <v>5660</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="2">
-        <v>45424.6875</v>
+        <v>45427.6875</v>
       </c>
       <c r="B68">
-        <v>4850</v>
+        <v>5700</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="2">
-        <v>45424.69791666666</v>
+        <v>45427.69791666666</v>
       </c>
       <c r="B69">
-        <v>4930</v>
+        <v>5770</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="2">
-        <v>45424.70833333334</v>
+        <v>45427.70833333334</v>
       </c>
       <c r="B70">
-        <v>5010</v>
+        <v>5890</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="2">
-        <v>45424.71875</v>
+        <v>45427.71875</v>
       </c>
       <c r="B71">
-        <v>5090</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="2">
-        <v>45424.72916666666</v>
+        <v>45427.72916666666</v>
       </c>
       <c r="B72">
-        <v>5190</v>
+        <v>6110</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="2">
-        <v>45424.73958333334</v>
+        <v>45427.73958333334</v>
       </c>
       <c r="B73">
-        <v>5290</v>
+        <v>6220</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="2">
-        <v>45424.75</v>
+        <v>45427.75</v>
       </c>
       <c r="B74">
-        <v>5400</v>
+        <v>6320</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="2">
-        <v>45424.76041666666</v>
+        <v>45427.76041666666</v>
       </c>
       <c r="B75">
-        <v>5510</v>
+        <v>6410</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="2">
-        <v>45424.77083333334</v>
+        <v>45427.77083333334</v>
       </c>
       <c r="B76">
-        <v>5630</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="2">
-        <v>45424.78125</v>
+        <v>45427.78125</v>
       </c>
       <c r="B77">
-        <v>5740</v>
+        <v>6600</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="2">
-        <v>45424.79166666666</v>
+        <v>45427.79166666666</v>
       </c>
       <c r="B78">
-        <v>5860</v>
+        <v>6700</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="2">
-        <v>45424.80208333334</v>
+        <v>45427.80208333334</v>
       </c>
       <c r="B79">
-        <v>5970</v>
+        <v>6810</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="2">
-        <v>45424.8125</v>
+        <v>45427.8125</v>
       </c>
       <c r="B80">
-        <v>6040</v>
+        <v>6910</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="2">
-        <v>45424.82291666666</v>
+        <v>45427.82291666666</v>
       </c>
       <c r="B81">
-        <v>6110</v>
+        <v>7040</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="2">
-        <v>45424.83333333334</v>
+        <v>45427.83333333334</v>
       </c>
       <c r="B82">
-        <v>6120</v>
+        <v>7130</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="2">
-        <v>45424.84375</v>
+        <v>45427.84375</v>
       </c>
       <c r="B83">
-        <v>6110</v>
+        <v>7130</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="2">
-        <v>45424.85416666666</v>
+        <v>45427.85416666666</v>
       </c>
       <c r="B84">
-        <v>6080</v>
+        <v>7120</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="2">
-        <v>45424.86458333334</v>
+        <v>45427.86458333334</v>
       </c>
       <c r="B85">
-        <v>6000</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="2">
-        <v>45424.875</v>
+        <v>45427.875</v>
       </c>
       <c r="B86">
-        <v>5870</v>
+        <v>6930</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="2">
-        <v>45424.88541666666</v>
+        <v>45427.88541666666</v>
       </c>
       <c r="B87">
-        <v>5750</v>
+        <v>6720</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="2">
-        <v>45424.89583333334</v>
+        <v>45427.89583333334</v>
       </c>
       <c r="B88">
-        <v>5620</v>
+        <v>6480</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="2">
-        <v>45424.90625</v>
+        <v>45427.90625</v>
       </c>
       <c r="B89">
-        <v>5490</v>
+        <v>6300</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="2">
-        <v>45424.91666666666</v>
+        <v>45427.91666666666</v>
       </c>
       <c r="B90">
-        <v>5360</v>
+        <v>6140</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" s="2">
-        <v>45424.92708333334</v>
+        <v>45427.92708333334</v>
       </c>
       <c r="B91">
-        <v>5240</v>
+        <v>6020</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" s="2">
-        <v>45424.9375</v>
+        <v>45427.9375</v>
       </c>
       <c r="B92">
-        <v>5130</v>
+        <v>5910</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="2">
-        <v>45424.94791666666</v>
+        <v>45427.94791666666</v>
       </c>
       <c r="B93">
-        <v>5020</v>
+        <v>5800</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" s="2">
-        <v>45424.95833333334</v>
+        <v>45427.95833333334</v>
       </c>
       <c r="B94">
-        <v>5050</v>
+        <v>5720</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="2">
-        <v>45424.96875</v>
+        <v>45427.96875</v>
       </c>
       <c r="B95">
-        <v>4990</v>
+        <v>5640</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" s="2">
-        <v>45424.97916666666</v>
+        <v>45427.97916666666</v>
       </c>
       <c r="B96">
-        <v>4930</v>
+        <v>5570</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="2">
-        <v>45424.98958333334</v>
+        <v>45427.98958333334</v>
       </c>
       <c r="B97">
-        <v>4880</v>
+        <v>5520</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" s="2">
-        <v>45425</v>
+        <v>45428</v>
       </c>
       <c r="B98">
-        <v>4840</v>
+        <v>5470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>